<commit_message>
more experiments with significantly fewer params
</commit_message>
<xml_diff>
--- a/results/siren_results.xlsx
+++ b/results/siren_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndebo\PycharmProjects\ImageCompression4k\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDACA535-99C5-4351-A6FD-A19F1A625695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9795CCE-6839-4F5A-B84D-FBB500A011E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="1935" windowWidth="24675" windowHeight="11265" xr2:uid="{6459C503-599E-47D2-879D-01B738E12182}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>siren</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>hidden layers</t>
+  </si>
+  <si>
+    <t>pixels</t>
+  </si>
+  <si>
+    <t>rgb nums</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBAFF8C0-ED42-4DCC-90FA-120C8907F36C}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +438,7 @@
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -460,8 +466,14 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>25</v>
       </c>
@@ -489,8 +501,16 @@
       <c r="I2">
         <v>256</v>
       </c>
+      <c r="J2">
+        <f>216*318</f>
+        <v>68688</v>
+      </c>
+      <c r="K2">
+        <f>J2*3</f>
+        <v>206064</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25</v>
       </c>
@@ -518,8 +538,16 @@
       <c r="I3">
         <v>256</v>
       </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J6" si="0">216*318</f>
+        <v>68688</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K6" si="1">J3*3</f>
+        <v>206064</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>25</v>
       </c>
@@ -546,9 +574,92 @@
       </c>
       <c r="I4">
         <v>256</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>68688</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>206064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>500</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>771</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.7336E-6</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>128</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>68688</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>206064</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.05</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>387</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4.7325E-6</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>64</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>68688</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>206064</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>